<commit_message>
Statistics for Factors Added
</commit_message>
<xml_diff>
--- a/DerivedData/MarkerStat.xlsx
+++ b/DerivedData/MarkerStat.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,60 +365,70 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Patients</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Sd</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CI Lower</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CI Upper</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Median</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Mad</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>IQR</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>50%</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>75%</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
@@ -431,39 +441,45 @@
         </is>
       </c>
       <c r="B2">
+        <v>2999</v>
+      </c>
+      <c r="C2">
+        <v>380</v>
+      </c>
+      <c r="D2">
         <v>100.08</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>58.12</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>41.96</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>158.2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>87</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>26.69</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>39</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>14</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>71</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>87</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>110</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>1236</v>
       </c>
     </row>
@@ -474,39 +490,45 @@
         </is>
       </c>
       <c r="B3">
+        <v>2999</v>
+      </c>
+      <c r="C3">
+        <v>380</v>
+      </c>
+      <c r="D3">
         <v>21.65</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>25.04</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>-3.390000000000001</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>46.69</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>7.41</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
       </c>
       <c r="J3">
         <v>12</v>
       </c>
       <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
         <v>17</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>24</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>966</v>
       </c>
     </row>
@@ -517,39 +539,45 @@
         </is>
       </c>
       <c r="B4">
+        <v>2989</v>
+      </c>
+      <c r="C4">
+        <v>380</v>
+      </c>
+      <c r="D4">
         <v>24.65</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>17.77</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>6.879999999999999</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>42.42</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>21</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>5.93</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>5</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>17</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>21</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>27</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>510</v>
       </c>
     </row>
@@ -560,39 +588,45 @@
         </is>
       </c>
       <c r="B5">
+        <v>2999</v>
+      </c>
+      <c r="C5">
+        <v>380</v>
+      </c>
+      <c r="D5">
         <v>86.28</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>25.67</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>60.61</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>111.95</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>82</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>20.76</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>26</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>27</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>71</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>82</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>97</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>560</v>
       </c>
     </row>
@@ -603,39 +637,45 @@
         </is>
       </c>
       <c r="B6">
+        <v>2989</v>
+      </c>
+      <c r="C6">
+        <v>380</v>
+      </c>
+      <c r="D6">
         <v>200.6</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>135.83</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>64.76999999999998</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>336.43</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>168</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>43</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>66</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>61</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>143</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>168</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>209</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>2610</v>
       </c>
     </row>
@@ -646,39 +686,45 @@
         </is>
       </c>
       <c r="B7">
+        <v>2905</v>
+      </c>
+      <c r="C7">
+        <v>380</v>
+      </c>
+      <c r="D7">
         <v>6.06</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>3.99</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>2.069999999999999</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>10.05</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>5.2</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>2.11</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>2.99</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>1.05</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>3.91</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>5.2</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>6.9</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>71.55</v>
       </c>
     </row>
@@ -689,39 +735,45 @@
         </is>
       </c>
       <c r="B8">
+        <v>2905</v>
+      </c>
+      <c r="C8">
+        <v>380</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>5.91</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>-0.3500000000000005</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>11.47</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>3.87</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>2.19</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>3.51</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>0.53</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>2.65</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>3.87</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>6.17</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>84.76000000000001</v>
       </c>
     </row>
@@ -732,39 +784,45 @@
         </is>
       </c>
       <c r="B9">
+        <v>1689</v>
+      </c>
+      <c r="C9">
+        <v>380</v>
+      </c>
+      <c r="D9">
         <v>7.47</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>5.82</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>1.649999999999999</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>13.29</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>4.45</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>6.5</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>3.5</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>6</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>44.4</v>
       </c>
     </row>
@@ -775,39 +833,45 @@
         </is>
       </c>
       <c r="B10">
+        <v>2908</v>
+      </c>
+      <c r="C10">
+        <v>380</v>
+      </c>
+      <c r="D10">
         <v>8.17</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>4.19</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>3.98</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>12.36</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>7.4</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>2.52</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>3.5</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>1.9</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>5.8</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>7.4</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>9.300000000000001</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>74.3</v>
       </c>
     </row>

</xml_diff>